<commit_message>
Fix bug in IsValid()
</commit_message>
<xml_diff>
--- a/ScriptTest1_Fixes.xlsx
+++ b/ScriptTest1_Fixes.xlsx
@@ -556,7 +556,7 @@
   <dimension ref="A1:N574"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -705,13 +705,22 @@
         <f aca="false">A4+1</f>
         <v>4</v>
       </c>
+      <c r="B5" s="1" t="n">
+        <v>41</v>
+      </c>
       <c r="D5" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C5)),(C5-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="G5" s="15" t="str">
+      <c r="E5" s="1" t="n">
+        <v>411</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="G5" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F5)),(F5-$N$2)/30, "")</f>
-        <v/>
+        <v>1.03333333333333</v>
       </c>
       <c r="J5" s="16"/>
     </row>
@@ -720,13 +729,22 @@
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
+      <c r="B6" s="1" t="n">
+        <v>411</v>
+      </c>
       <c r="D6" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C6)),(C6-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="G6" s="15" t="str">
+      <c r="E6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="G6" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F6)),(F6-$N$2)/30, "")</f>
-        <v/>
+        <v>1.06666666666667</v>
       </c>
       <c r="J6" s="16"/>
     </row>

</xml_diff>

<commit_message>
Add more testing data
</commit_message>
<xml_diff>
--- a/ScriptTest1_Fixes.xlsx
+++ b/ScriptTest1_Fixes.xlsx
@@ -556,7 +556,7 @@
   <dimension ref="A1:N574"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,13 +753,22 @@
         <f aca="false">A6+1</f>
         <v>6</v>
       </c>
+      <c r="B7" s="1" t="n">
+        <v>11</v>
+      </c>
       <c r="D7" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C7)),(C7-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="G7" s="15" t="str">
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F7)),(F7-$N$2)/30, "")</f>
-        <v/>
+        <v>0.166666666666667</v>
       </c>
       <c r="J7" s="16"/>
     </row>
@@ -768,13 +777,22 @@
         <f aca="false">A7+1</f>
         <v>7</v>
       </c>
+      <c r="B8" s="1" t="n">
+        <v>42</v>
+      </c>
       <c r="D8" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C8)),(C8-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="G8" s="15" t="str">
+      <c r="E8" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="G8" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F8)),(F8-$N$2)/30, "")</f>
-        <v/>
+        <v>1.1</v>
       </c>
       <c r="J8" s="16"/>
     </row>
@@ -783,13 +801,22 @@
         <f aca="false">A8+1</f>
         <v>8</v>
       </c>
+      <c r="B9" s="1" t="n">
+        <v>88</v>
+      </c>
       <c r="D9" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C9)),(C9-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="G9" s="15" t="str">
+      <c r="E9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="G9" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F9)),(F9-$N$2)/30, "")</f>
-        <v/>
+        <v>2.33333333333333</v>
       </c>
       <c r="J9" s="16"/>
     </row>
@@ -798,13 +825,22 @@
         <f aca="false">A9+1</f>
         <v>9</v>
       </c>
+      <c r="B10" s="1" t="n">
+        <v>888</v>
+      </c>
       <c r="D10" s="14" t="str">
         <f aca="false">IF(NOT(ISBLANK(C10)),(C10-$N$2)/30, "")</f>
         <v/>
       </c>
-      <c r="G10" s="15" t="str">
+      <c r="E10" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="G10" s="15" t="n">
         <f aca="false">IF(NOT(ISBLANK(F10)),(F10-$N$2)/30, "")</f>
-        <v/>
+        <v>2.5</v>
       </c>
       <c r="J10" s="16"/>
     </row>

</xml_diff>